<commit_message>
add area to Q files stn3
</commit_message>
<xml_diff>
--- a/Discharge/Station3_2021-06-25_1230.xlsx
+++ b/Discharge/Station3_2021-06-25_1230.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efarq\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1cba20500feb7d90/Documents/LongTermData_CayambeCoca/Discharge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8F5F124-CF94-4AB5-8EE9-2434379E7780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{A8F5F124-CF94-4AB5-8EE9-2434379E7780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70561187-A04A-4667-841A-335D2884B075}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1070" windowWidth="14640" windowHeight="9730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>x</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Qtotal</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Atotal</t>
   </si>
 </sst>
 </file>
@@ -369,15 +375,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="J2" sqref="J2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -396,8 +402,20 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>50</v>
       </c>
@@ -409,8 +427,24 @@
         <f>SUM(E2:E20)</f>
         <v>7.064E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2">
+        <f>(D2-0)*B2/100</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>SUM(G2:G11)</f>
+        <v>2.2700000000000001E-2</v>
+      </c>
+      <c r="J2">
+        <f>H2</f>
+        <v>2.2700000000000001E-2</v>
+      </c>
+      <c r="K2">
+        <f>F2</f>
+        <v>7.064E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>55</v>
       </c>
@@ -428,8 +462,12 @@
         <f>(D3-D2)*(B3/100)*C3</f>
         <v>4.0799999999999978E-4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <f>(D3-D2)*B3/100</f>
+        <v>3.3999999999999985E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>62</v>
       </c>
@@ -444,11 +482,15 @@
         <v>0.63</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E12" si="0">(D4-D3)*(B4/100)*C4</f>
+        <f t="shared" ref="E4:E9" si="0">(D4-D3)*(B4/100)*C4</f>
         <v>7.4250000000000065E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <f t="shared" ref="G4:G15" si="1">(D4-D3)*B4/100</f>
+        <v>2.250000000000002E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>64</v>
       </c>
@@ -466,8 +508,12 @@
         <f>(D5-D4)*(B5/100)*C5</f>
         <v>1.8900000000000019E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>4.2000000000000041E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>68</v>
       </c>
@@ -478,15 +524,19 @@
         <v>0.4</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D12" si="1">(A6/100+(A7/100-A6/100)/2)</f>
+        <f t="shared" ref="D6:D9" si="2">(A6/100+(A7/100-A6/100)/2)</f>
         <v>0.69</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
         <v>1.6799999999999955E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>4.1999999999999885E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>70</v>
       </c>
@@ -497,15 +547,19 @@
         <v>0.34</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.72</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
         <v>1.2240000000000011E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>3.6000000000000034E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>74</v>
       </c>
@@ -516,15 +570,19 @@
         <v>0.23</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.77</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
         <v>9.200000000000009E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>80</v>
       </c>
@@ -535,17 +593,55 @@
         <v>0.19</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.80500000000000005</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
         <v>1.9950000000000016E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>1.050000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>81</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>